<commit_message>
new analyse result ,bad!!
</commit_message>
<xml_diff>
--- a/analyse_result.xlsx
+++ b/analyse_result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wangwensong\Desktop\Low-res_cryo-EM_comparable_high_res_X-ray\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{470C96C4-060F-4AD0-AFB5-FA2E810A9A84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{213677F5-0F36-423E-9624-A28DD35512C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,6 @@
     <sheet name="6o1m" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="48">
   <si>
     <t>bond_rms</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -91,10 +90,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2.08/11.46/86.46</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">method  </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -111,10 +106,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2.98/22.98/74.04</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0.91/7.65/91.44</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -192,6 +183,45 @@
   </si>
   <si>
     <t>0/5.86/94.14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>geo_mini</t>
+  </si>
+  <si>
+    <t>geo_mini</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.07/13.36/84.57</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.17/2.08/93.75</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.78/5.99/93.23</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.43/11.34/88.23</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.27/9.90/89.93</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.16/13.26/85.58</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.24/13.11/85.65</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.82/12.66/85.52</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -519,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="A1:H5"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -533,7 +563,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -643,22 +673,48 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="C5">
-        <v>1.58</v>
+        <v>1.216</v>
       </c>
       <c r="D5">
-        <v>35.18</v>
+        <v>21.98</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F5" s="1">
-        <v>0.2024</v>
-      </c>
-      <c r="G5" s="1">
-        <v>1.09E-2</v>
+        <v>0.21429999999999999</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>-4.165</v>
+        <v>-5.8479999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6">
+        <v>1E-3</v>
+      </c>
+      <c r="C6">
+        <v>0.23699999999999999</v>
+      </c>
+      <c r="D6">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>-2.081</v>
       </c>
     </row>
   </sheetData>
@@ -670,10 +726,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DE795C8-0411-4F0F-9C5C-E071F277445F}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H5"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -685,7 +741,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -723,7 +779,7 @@
         <v>0.97</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F2" s="1">
         <v>4.0500000000000001E-2</v>
@@ -749,7 +805,7 @@
         <v>65.98</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" s="1">
         <v>0.10580000000000001</v>
@@ -775,7 +831,7 @@
         <v>59.17</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4" s="1">
         <v>5.7700000000000001E-2</v>
@@ -792,25 +848,51 @@
         <v>13</v>
       </c>
       <c r="B5">
-        <v>1.9E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="C5">
-        <v>2.9820000000000002</v>
+        <v>2.7959999999999998</v>
       </c>
       <c r="D5">
-        <v>90.57</v>
+        <v>65.98</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F5" s="1">
-        <v>0.14899999999999999</v>
+        <v>0.10580000000000001</v>
       </c>
       <c r="G5" s="1">
-        <v>2.18E-2</v>
+        <v>1.3100000000000001E-2</v>
       </c>
       <c r="H5">
-        <v>-5.6109999999999998</v>
+        <v>-5.6079999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6">
+        <v>1E-3</v>
+      </c>
+      <c r="C6">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="D6">
+        <v>0.93</v>
+      </c>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.52</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>-2.754</v>
       </c>
     </row>
   </sheetData>
@@ -821,10 +903,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{676488E4-98E9-433F-B5B9-8F87A653AD1D}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -836,7 +918,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -874,7 +956,7 @@
         <v>4.47</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F2" s="1">
         <v>5.9999999999999995E-4</v>
@@ -900,7 +982,7 @@
         <v>48.92</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F3" s="1">
         <v>5.1299999999999998E-2</v>
@@ -926,7 +1008,7 @@
         <v>39.229999999999997</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F4" s="1">
         <v>1.3299999999999999E-2</v>
@@ -952,7 +1034,7 @@
         <v>48.92</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F5" s="1">
         <v>5.1299999999999998E-2</v>
@@ -962,6 +1044,32 @@
       </c>
       <c r="H5">
         <v>-3.9710000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6">
+        <v>1E-3</v>
+      </c>
+      <c r="C6">
+        <v>0.32600000000000001</v>
+      </c>
+      <c r="D6">
+        <v>3.04</v>
+      </c>
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>-3.585</v>
       </c>
     </row>
   </sheetData>
@@ -973,10 +1081,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B241A5E2-7B2C-4241-BAE3-6B5B36FED694}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -987,7 +1095,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1025,7 +1133,7 @@
         <v>1.23</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F2" s="1">
         <v>0</v>
@@ -1051,7 +1159,7 @@
         <v>5.25</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F3" s="1">
         <v>2.0899999999999998E-2</v>
@@ -1077,7 +1185,7 @@
         <v>4.67</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4" s="1">
         <v>5.7000000000000002E-3</v>
@@ -1103,7 +1211,7 @@
         <v>14.7</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F5" s="1">
         <v>2.47E-2</v>
@@ -1113,6 +1221,32 @@
       </c>
       <c r="H5">
         <v>-3.5609999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6">
+        <v>1E-3</v>
+      </c>
+      <c r="C6">
+        <v>0.33</v>
+      </c>
+      <c r="D6">
+        <v>2.29</v>
+      </c>
+      <c r="E6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>-3.347</v>
       </c>
     </row>
   </sheetData>
@@ -1123,10 +1257,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC735A71-DB35-4C7D-AF3C-E14313B08658}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1137,7 +1271,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1175,7 +1309,7 @@
         <v>7.41</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F2" s="1">
         <v>0</v>
@@ -1201,7 +1335,7 @@
         <v>9.8800000000000008</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F3" s="1">
         <v>1.2E-2</v>
@@ -1227,7 +1361,7 @@
         <v>7.69</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F4" s="1">
         <v>0</v>
@@ -1253,7 +1387,7 @@
         <v>28.69</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F5" s="1">
         <v>2.29E-2</v>
@@ -1263,6 +1397,32 @@
       </c>
       <c r="H5">
         <v>-4.673</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6">
+        <v>1E-3</v>
+      </c>
+      <c r="C6">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="D6">
+        <v>3.57</v>
+      </c>
+      <c r="E6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1.2E-2</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>-4.1100000000000003</v>
       </c>
     </row>
   </sheetData>
@@ -1273,10 +1433,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D02A25A1-8944-4273-8123-EA18BDD43F63}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1288,7 +1448,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1326,7 +1486,7 @@
         <v>4.54</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F2" s="1">
         <v>1.6999999999999999E-3</v>
@@ -1352,7 +1512,7 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F3" s="1">
         <v>4.8399999999999999E-2</v>
@@ -1378,7 +1538,7 @@
         <v>4.8899999999999997</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F4" s="1">
         <v>1.5800000000000002E-2</v>
@@ -1404,7 +1564,7 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F5" s="1">
         <v>4.8399999999999999E-2</v>
@@ -1414,6 +1574,32 @@
       </c>
       <c r="H5">
         <v>-2.919</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6">
+        <v>1E-3</v>
+      </c>
+      <c r="C6">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="D6">
+        <v>3.88</v>
+      </c>
+      <c r="E6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="1">
+        <v>4.1999999999999997E-3</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>-3.6179999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -1424,10 +1610,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4148CA6-2904-4197-957E-F2396D22A0D2}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1439,7 +1625,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1477,7 +1663,7 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F2" s="1">
         <v>1.2E-2</v>
@@ -1503,7 +1689,7 @@
         <v>9.5399999999999991</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F3" s="1">
         <v>6.83E-2</v>
@@ -1529,7 +1715,7 @@
         <v>7.11</v>
       </c>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F4" s="1">
         <v>3.5900000000000001E-2</v>
@@ -1555,7 +1741,7 @@
         <v>9.5399999999999991</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F5" s="1">
         <v>6.83E-2</v>
@@ -1565,6 +1751,32 @@
       </c>
       <c r="H5">
         <v>-3.762</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6">
+        <v>1E-3</v>
+      </c>
+      <c r="C6">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="D6">
+        <v>3.69</v>
+      </c>
+      <c r="E6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="1">
+        <v>4.8999999999999998E-3</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>-3.891</v>
       </c>
     </row>
   </sheetData>
@@ -1575,10 +1787,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A1628F3-807D-4B8A-85E6-453AE74A0899}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1590,7 +1802,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1628,7 +1840,7 @@
         <v>5.71</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F2" s="1">
         <v>5.4999999999999997E-3</v>
@@ -1654,7 +1866,7 @@
         <v>8.5399999999999991</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F3" s="1">
         <v>7.4999999999999997E-2</v>
@@ -1680,7 +1892,7 @@
         <v>7.61</v>
       </c>
       <c r="E4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F4" s="1">
         <v>2.93E-2</v>
@@ -1706,7 +1918,7 @@
         <v>8.5399999999999991</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F5" s="1">
         <v>7.4999999999999997E-2</v>
@@ -1716,6 +1928,32 @@
       </c>
       <c r="H5">
         <v>-3.6190000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6">
+        <v>1E-3</v>
+      </c>
+      <c r="C6">
+        <v>0.33200000000000002</v>
+      </c>
+      <c r="D6">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="E6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="1">
+        <v>6.1000000000000004E-3</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>-3.7930000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>